<commit_message>
order eims rows & add ncp student creators
</commit_message>
<xml_diff>
--- a/ncp-gop-transect-2018-pkg13/ncp-gop-transect-info.xlsx
+++ b/ncp-gop-transect-2018-pkg13/ncp-gop-transect-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-eims-toi-ncp-gop\ncp-gop-transect-2018-pkg13\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC09FD23-B9BC-4F53-A20D-5D49CFC3A609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DEFA94-E713-4BFB-BAC6-14B3A1440D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="21384" windowHeight="11424" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeadersGop" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="121">
   <si>
     <t>givenName</t>
   </si>
@@ -378,6 +378,21 @@
   </si>
   <si>
     <t xml:space="preserve"> H R</t>
+  </si>
+  <si>
+    <t>Arshia</t>
+  </si>
+  <si>
+    <t>Mehta</t>
+  </si>
+  <si>
+    <t>amehta3@wellesley.edu</t>
+  </si>
+  <si>
+    <t>Aldrett</t>
+  </si>
+  <si>
+    <t>Danielle</t>
   </si>
 </sst>
 </file>
@@ -1236,10 +1251,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B5"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1481,6 +1496,55 @@
         <v>12</v>
       </c>
       <c r="J8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>118</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" t="s">
+        <v>119</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>